<commit_message>
Added Oppressor Mk II request and adjusted some minor settings.
</commit_message>
<xml_diff>
--- a/Macro Quick Reference.xlsx
+++ b/Macro Quick Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8698d8018a0031f0/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Mods\gtav-online-ahk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{C0E4385D-130A-49B7-9BF9-1D4AD0AC21FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{237F350F-33B9-4814-B30E-BE3533ABB549}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E351DA-A427-49F8-9E0C-3BC0ADD77D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43118" yWindow="0" windowWidth="14565" windowHeight="15563" xr2:uid="{16D26845-CD69-4375-957C-84A1F5A933EA}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{16D26845-CD69-4375-957C-84A1F5A933EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Key</t>
   </si>
@@ -231,13 +231,19 @@
   </si>
   <si>
     <t>New Public Session</t>
+  </si>
+  <si>
+    <t>+F4</t>
+  </si>
+  <si>
+    <t>Request Oppressor Mk II</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,18 +662,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CABBABCD-4338-4956-AC97-03A985E7BE7A}">
-  <dimension ref="A1:AA41"/>
+  <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="8.59765625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="30.73046875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.06640625" customWidth="1"/>
+    <col min="1" max="1" width="8.625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="30.75" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.0625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -704,7 +712,7 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -741,7 +749,7 @@
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
     </row>
-    <row r="3" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -778,7 +786,7 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
     </row>
-    <row r="4" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
@@ -811,7 +819,7 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -844,7 +852,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -877,7 +885,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -910,7 +918,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
@@ -943,7 +951,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -976,12 +984,12 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1009,12 +1017,12 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1042,12 +1050,12 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A12" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1075,12 +1083,12 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="13" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A13" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1108,12 +1116,12 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
     </row>
-    <row r="14" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A14" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1141,12 +1149,12 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A15" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1174,12 +1182,12 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1207,12 +1215,12 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
     </row>
-    <row r="17" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1240,12 +1248,12 @@
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
     </row>
-    <row r="18" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A18" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1273,12 +1281,12 @@
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
     </row>
-    <row r="19" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A19" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1306,12 +1314,12 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
-    <row r="20" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A20" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1339,12 +1347,12 @@
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
-    <row r="21" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A21" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1372,12 +1380,12 @@
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A22" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1405,12 +1413,12 @@
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
-    <row r="23" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A23" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1438,12 +1446,12 @@
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1471,12 +1479,12 @@
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
     </row>
-    <row r="25" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1504,12 +1512,12 @@
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
     </row>
-    <row r="26" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A26" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -1537,12 +1545,12 @@
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
     </row>
-    <row r="27" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A27" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1570,12 +1578,12 @@
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
     </row>
-    <row r="28" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A28" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1603,12 +1611,12 @@
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A29" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1636,12 +1644,12 @@
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
       <c r="A30" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1669,9 +1677,13 @@
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="2"/>
-      <c r="B31" s="3"/>
+    <row r="31" spans="1:27" ht="18.399999999999999" thickTop="1" thickBot="1">
+      <c r="A31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1698,7 +1710,7 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="1"/>
@@ -1727,7 +1739,7 @@
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A33" s="2"/>
       <c r="B33" s="3"/>
       <c r="C33" s="1"/>
@@ -1756,7 +1768,7 @@
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
     </row>
-    <row r="34" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A34" s="2"/>
       <c r="B34" s="3"/>
       <c r="C34" s="1"/>
@@ -1785,7 +1797,7 @@
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
     </row>
-    <row r="35" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A35" s="2"/>
       <c r="B35" s="3"/>
       <c r="C35" s="1"/>
@@ -1814,7 +1826,7 @@
       <c r="Z35" s="1"/>
       <c r="AA35" s="1"/>
     </row>
-    <row r="36" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="1"/>
@@ -1843,7 +1855,7 @@
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
     </row>
-    <row r="37" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A37" s="2"/>
       <c r="B37" s="3"/>
       <c r="C37" s="1"/>
@@ -1872,7 +1884,7 @@
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
     </row>
-    <row r="38" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A38" s="2"/>
       <c r="B38" s="3"/>
       <c r="C38" s="1"/>
@@ -1901,7 +1913,7 @@
       <c r="Z38" s="1"/>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="1"/>
@@ -1930,7 +1942,7 @@
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" spans="1:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
       <c r="A40" s="2"/>
       <c r="B40" s="3"/>
       <c r="C40" s="1"/>
@@ -1959,7 +1971,36 @@
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
     </row>
-    <row r="41" spans="1:27" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="41" spans="1:27" ht="14.65" thickTop="1" thickBot="1">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1"/>
+      <c r="Y41" s="1"/>
+      <c r="Z41" s="1"/>
+      <c r="AA41" s="1"/>
+    </row>
+    <row r="42" spans="1:27" ht="13.9" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>